<commit_message>
add other nzte datasets
</commit_message>
<xml_diff>
--- a/parse_nzte_stockable/_Appendix.C_Full.detail.stocktake.xlsx
+++ b/parse_nzte_stockable/_Appendix.C_Full.detail.stocktake.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quentint/Desktop/parse_koray_atalag_list/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quentint/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1380" windowWidth="36300" windowHeight="17540"/>
+    <workbookView xWindow="-38400" yWindow="-2940" windowWidth="38400" windowHeight="22280"/>
   </bookViews>
   <sheets>
     <sheet name="Intv.form_sort.20130628" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3808" uniqueCount="1320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4314" uniqueCount="1422">
   <si>
     <t>DataSet(s)</t>
   </si>
@@ -4126,6 +4126,312 @@
   </si>
   <si>
     <t>tags_</t>
+  </si>
+  <si>
+    <t>http://www.ash.org.nz/</t>
+  </si>
+  <si>
+    <t>Action on Smoking and Health</t>
+  </si>
+  <si>
+    <t>Australian and New Zealand Society of Cardiac and Thoracic Surgeons</t>
+  </si>
+  <si>
+    <t>https://anzscts.org/</t>
+  </si>
+  <si>
+    <t>http://www.researchnz.com/</t>
+  </si>
+  <si>
+    <t>Research New Zealand</t>
+  </si>
+  <si>
+    <t>alcohol|addiction</t>
+  </si>
+  <si>
+    <t>http://www.midlandcancernetwork.org.nz/</t>
+  </si>
+  <si>
+    <t>Midland Cancer Network</t>
+  </si>
+  <si>
+    <t>https://www.sialliance.health.nz/our-priorities/southern-cancer-network/</t>
+  </si>
+  <si>
+    <t>Southern Cancer Network</t>
+  </si>
+  <si>
+    <t>cancer|oncology|pulmonology</t>
+  </si>
+  <si>
+    <t>cancer|oncology|gastroenterology</t>
+  </si>
+  <si>
+    <t>Canterbury and West Coast District Health Board</t>
+  </si>
+  <si>
+    <t>http://www.westcoastdhb.org.nz/</t>
+  </si>
+  <si>
+    <t>emergency|hospital</t>
+  </si>
+  <si>
+    <t>inpatient|hospital</t>
+  </si>
+  <si>
+    <t>outpatient|hospital</t>
+  </si>
+  <si>
+    <t>waiting-time|hospital</t>
+  </si>
+  <si>
+    <t>rehabilitation|hospital</t>
+  </si>
+  <si>
+    <t>mental-health|hospital</t>
+  </si>
+  <si>
+    <t>hospital|referral</t>
+  </si>
+  <si>
+    <t>medication</t>
+  </si>
+  <si>
+    <t>medication|hospital</t>
+  </si>
+  <si>
+    <t>ambulance|hospital</t>
+  </si>
+  <si>
+    <t>elderly|hospital</t>
+  </si>
+  <si>
+    <t>pediatrics|hospital</t>
+  </si>
+  <si>
+    <t>image|hospital</t>
+  </si>
+  <si>
+    <t>lifestyle|nutrition|smoking|tobacco|addiction</t>
+  </si>
+  <si>
+    <t>http://www.cbg.co.nz/</t>
+  </si>
+  <si>
+    <t>http://www.dpt.org.nz/</t>
+  </si>
+  <si>
+    <t>new-zealand labs-and-imaging-centres</t>
+  </si>
+  <si>
+    <t>http://www.dml.co.nz/</t>
+  </si>
+  <si>
+    <t>Diagnostic Medical Laboratory</t>
+  </si>
+  <si>
+    <t>https://www.drinfo.co.nz/</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>http://www.enigma.co.nz/2015/12/23/predict-enigma-view-university-of-auckland-looking-forward-to-2016/</t>
+  </si>
+  <si>
+    <t>Enigma</t>
+  </si>
+  <si>
+    <t>http://www.esr.cri.nz/</t>
+  </si>
+  <si>
+    <t>Institute of Environmental Science and Research</t>
+  </si>
+  <si>
+    <t>sti</t>
+  </si>
+  <si>
+    <t>disease</t>
+  </si>
+  <si>
+    <t>http://www.flinders.edu.au/medicine/sites/ophthalmology/clinical/aus-nz-registry-of-advanced-glaucoma.cfm</t>
+  </si>
+  <si>
+    <t>ophthalmology</t>
+  </si>
+  <si>
+    <t>http://www.growingup.co.nz/en/access-to-guinz-data.html</t>
+  </si>
+  <si>
+    <t>Growing up in New Zealand</t>
+  </si>
+  <si>
+    <t>dermatology|sun</t>
+  </si>
+  <si>
+    <t>http://www.hpa.org.nz/</t>
+  </si>
+  <si>
+    <t>(ex) Health Sponsorship Council</t>
+  </si>
+  <si>
+    <t>Pharmaceutical Management Agency</t>
+  </si>
+  <si>
+    <t>medication|pharmacy</t>
+  </si>
+  <si>
+    <t>Genetic Health Service NZ</t>
+  </si>
+  <si>
+    <t>http://www.genetichealthservice.org.nz/</t>
+  </si>
+  <si>
+    <t>genetics</t>
+  </si>
+  <si>
+    <t>https://www.plunket.org.nz/</t>
+  </si>
+  <si>
+    <t>new-zealand primary-community-care-providers</t>
+  </si>
+  <si>
+    <t>bioengineering</t>
+  </si>
+  <si>
+    <t>https://metrosouth.health.qld.gov.au/princess-alexandra-hospital</t>
+  </si>
+  <si>
+    <t>https://www.nzma.org.nz/journal/read-the-journal/all-issues/2010-2019/2016/vol-129-no-1439-5-august-2016/6959</t>
+  </si>
+  <si>
+    <t>New Zealand Social Science Data Service</t>
+  </si>
+  <si>
+    <t>http://www.nzssn.org.nz/</t>
+  </si>
+  <si>
+    <t>http://www.northerncancernetwork.org.nz/</t>
+  </si>
+  <si>
+    <t>Northern Cancer Network</t>
+  </si>
+  <si>
+    <t>http://www.whanautahi.com/</t>
+  </si>
+  <si>
+    <t>(ex) HSA Global</t>
+  </si>
+  <si>
+    <t>http://www.healthalliance.co.nz/</t>
+  </si>
+  <si>
+    <t>laboratory|radiology|pharmacy</t>
+  </si>
+  <si>
+    <t>rheumatology</t>
+  </si>
+  <si>
+    <t>https://www.auckland.ac.nz/en.html</t>
+  </si>
+  <si>
+    <t>http://www.labtests.co.nz/</t>
+  </si>
+  <si>
+    <t>laboratory|image</t>
+  </si>
+  <si>
+    <t>individual Primary Health Organizations</t>
+  </si>
+  <si>
+    <t>primary-care|claim</t>
+  </si>
+  <si>
+    <t>https://www.nursemaude.org.nz/</t>
+  </si>
+  <si>
+    <t>nurse|home-care</t>
+  </si>
+  <si>
+    <t>https://www.medibankhealth.com.au/</t>
+  </si>
+  <si>
+    <t>Medibank Health Solutions</t>
+  </si>
+  <si>
+    <t>https://www.auckland.ac.nz/</t>
+  </si>
+  <si>
+    <t>blood-donation</t>
+  </si>
+  <si>
+    <t>tobacco|smoking|addiction</t>
+  </si>
+  <si>
+    <t>cholesterol</t>
+  </si>
+  <si>
+    <t>stroke</t>
+  </si>
+  <si>
+    <t>tobacco|smoking|cardiology</t>
+  </si>
+  <si>
+    <t>tobacco|smoking|addiction|alcohol</t>
+  </si>
+  <si>
+    <t>car-crash</t>
+  </si>
+  <si>
+    <t>sleep</t>
+  </si>
+  <si>
+    <t>ulcer|medication</t>
+  </si>
+  <si>
+    <t>sport|global-health</t>
+  </si>
+  <si>
+    <t>asthma</t>
+  </si>
+  <si>
+    <t>research</t>
+  </si>
+  <si>
+    <t>social|research</t>
+  </si>
+  <si>
+    <t>social|research|qol|lifstyle</t>
+  </si>
+  <si>
+    <t>barthel-index|research|adl</t>
+  </si>
+  <si>
+    <t>qol|research|cardiology</t>
+  </si>
+  <si>
+    <t>freemasons|research</t>
+  </si>
+  <si>
+    <t>steroid|research</t>
+  </si>
+  <si>
+    <t>qol|research</t>
+  </si>
+  <si>
+    <t>radiology|research</t>
+  </si>
+  <si>
+    <t>adherence|research</t>
+  </si>
+  <si>
+    <t>nutrition|research</t>
+  </si>
+  <si>
+    <t>addiction|research</t>
+  </si>
+  <si>
+    <t>sport|lifestyle|research</t>
   </si>
 </sst>
 </file>
@@ -4493,14 +4799,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:W287"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="124" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B215" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U1" sqref="U1"/>
+      <selection pane="bottomRight" activeCell="F286" sqref="F286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4590,7 +4895,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="156" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" ht="156" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -8013,16 +8318,25 @@
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:23" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:23" ht="60" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>236</v>
       </c>
+      <c r="B62" s="1" t="s">
+        <v>1369</v>
+      </c>
       <c r="C62" s="1" t="s">
         <v>1170</v>
       </c>
+      <c r="D62" s="1" t="s">
+        <v>1175</v>
+      </c>
       <c r="E62" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>|nzte-report</v>
+        <v>medication|pharmacy|nzte-report</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>1370</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>19</v>
@@ -8073,16 +8387,25 @@
         <v>246</v>
       </c>
     </row>
-    <row r="63" spans="1:23" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:23" ht="60" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>247</v>
       </c>
+      <c r="B63" s="1" t="s">
+        <v>1369</v>
+      </c>
       <c r="C63" s="1" t="s">
         <v>1170</v>
       </c>
+      <c r="D63" s="1" t="s">
+        <v>1175</v>
+      </c>
       <c r="E63" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>|nzte-report</v>
+        <v>medication|hospital|nzte-report</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>1343</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>19</v>
@@ -8259,13 +8582,25 @@
         <v>270</v>
       </c>
     </row>
-    <row r="66" spans="1:23" ht="90" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:23" ht="90" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>271</v>
       </c>
+      <c r="B66" s="1" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>1372</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>1230</v>
+      </c>
       <c r="E66" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>|nzte-report</v>
+        <v>genetics|nzte-report</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>1373</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>258</v>
@@ -9075,13 +9410,25 @@
         <v>55</v>
       </c>
     </row>
-    <row r="81" spans="1:23" ht="225" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:23" ht="225" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>379</v>
       </c>
+      <c r="B81" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>1375</v>
+      </c>
       <c r="E81" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>pediatrics|nzte-report</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>1184</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>380</v>
@@ -9132,13 +9479,25 @@
         <v>392</v>
       </c>
     </row>
-    <row r="82" spans="1:23" ht="120" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:23" ht="120" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>393</v>
       </c>
+      <c r="B82" s="1" t="s">
+        <v>1359</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E82" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>sti|nzte-report</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>1360</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>394</v>
@@ -9189,13 +9548,25 @@
         <v>407</v>
       </c>
     </row>
-    <row r="83" spans="1:23" ht="90" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:23" ht="90" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>408</v>
       </c>
+      <c r="B83" s="1" t="s">
+        <v>1359</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E83" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>laboratory|nzte-report</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>1237</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>394</v>
@@ -9246,13 +9617,25 @@
         <v>407</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="165" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:23" ht="165" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>416</v>
       </c>
+      <c r="B84" s="1" t="s">
+        <v>1359</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E84" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>disease|nzte-report</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>1361</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>394</v>
@@ -9360,16 +9743,25 @@
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:23" ht="75" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>431</v>
       </c>
+      <c r="B86" s="1" t="s">
+        <v>432</v>
+      </c>
       <c r="C86" s="1" t="s">
         <v>1171</v>
       </c>
+      <c r="D86" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E86" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>bioengineering|nzte-report</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>1376</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>394</v>
@@ -9423,13 +9815,25 @@
         <v>442</v>
       </c>
     </row>
-    <row r="87" spans="1:23" ht="240" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:23" ht="240" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>443</v>
       </c>
+      <c r="B87" s="1" t="s">
+        <v>1322</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>1256</v>
+      </c>
       <c r="E87" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>cardiology|nzte-report</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>1205</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>444</v>
@@ -9480,13 +9884,25 @@
         <v>455</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="90" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:23" ht="90" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>456</v>
       </c>
+      <c r="B88" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>1256</v>
+      </c>
       <c r="E88" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>nephrology|nzte-report</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>1315</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>444</v>
@@ -9501,13 +9917,25 @@
         <v>456</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:23" ht="60" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>458</v>
       </c>
+      <c r="B89" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>1362</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>1256</v>
+      </c>
       <c r="E89" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>ophthalmology|nzte-report</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>1363</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>444</v>
@@ -9864,13 +10292,25 @@
         <v>81</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="180" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:23" ht="180" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>476</v>
       </c>
+      <c r="B96" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>1377</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>1256</v>
+      </c>
       <c r="E96" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>nephrology|nzte-report</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>1315</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>444</v>
@@ -9924,13 +10364,25 @@
         <v>490</v>
       </c>
     </row>
-    <row r="97" spans="1:23" ht="210" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:23" ht="210" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>491</v>
       </c>
+      <c r="B97" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>1378</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>1256</v>
+      </c>
       <c r="E97" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>cardiology|nzte-report</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>1205</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>444</v>
@@ -9981,13 +10433,25 @@
         <v>502</v>
       </c>
     </row>
-    <row r="98" spans="1:23" ht="150" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:23" ht="150" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>503</v>
       </c>
+      <c r="B98" s="1" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>1320</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>1257</v>
+      </c>
       <c r="E98" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>tobacco|smoking|nzte-report</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>1287</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>504</v>
@@ -10038,13 +10502,25 @@
         <v>513</v>
       </c>
     </row>
-    <row r="99" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>514</v>
       </c>
+      <c r="B99" s="1" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>1320</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>1257</v>
+      </c>
       <c r="E99" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>tobacco|smoking|nzte-report</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>1287</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>504</v>
@@ -10083,13 +10559,25 @@
         <v>187</v>
       </c>
     </row>
-    <row r="100" spans="1:23" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:23" ht="60" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>517</v>
       </c>
+      <c r="B100" s="1" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>1257</v>
+      </c>
       <c r="E100" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>alcohol|addiction|nzte-report</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>1326</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>504</v>
@@ -10128,13 +10616,25 @@
         <v>513</v>
       </c>
     </row>
-    <row r="101" spans="1:23" ht="75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:23" ht="75" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>520</v>
       </c>
+      <c r="B101" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>1257</v>
+      </c>
       <c r="E101" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>lifestyle|nutrition|smoking|tobacco|addiction|nzte-report</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>1348</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>504</v>
@@ -10176,13 +10676,25 @@
         <v>513</v>
       </c>
     </row>
-    <row r="102" spans="1:23" ht="180" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:23" ht="180" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>526</v>
       </c>
+      <c r="B102" s="1" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>1257</v>
+      </c>
       <c r="E102" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>tobacco|smoking|nzte-report</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>1287</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>504</v>
@@ -10215,13 +10727,25 @@
         <v>529</v>
       </c>
     </row>
-    <row r="103" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:23" ht="45" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>530</v>
       </c>
+      <c r="B103" s="1" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>1257</v>
+      </c>
       <c r="E103" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>dermatology|sun|nzte-report</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>1366</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>504</v>
@@ -10260,13 +10784,25 @@
         <v>513</v>
       </c>
     </row>
-    <row r="104" spans="1:23" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:23" ht="60" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>534</v>
       </c>
+      <c r="B104" s="1" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>1257</v>
+      </c>
       <c r="E104" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>tobacco|smoking|nzte-report</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>1287</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>504</v>
@@ -11646,13 +12182,25 @@
         <v>624</v>
       </c>
     </row>
-    <row r="129" spans="1:23" ht="240" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:23" ht="240" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>625</v>
       </c>
+      <c r="B129" s="1" t="s">
+        <v>1379</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>1380</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>1257</v>
+      </c>
       <c r="E129" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>primary-care|nzte-report</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>1214</v>
       </c>
       <c r="G129" s="1" t="s">
         <v>504</v>
@@ -11670,13 +12218,25 @@
         <v>628</v>
       </c>
     </row>
-    <row r="130" spans="1:23" ht="409" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:23" ht="409" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>629</v>
       </c>
+      <c r="B130" s="1" t="s">
+        <v>1328</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>1327</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>1175</v>
+      </c>
       <c r="E130" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>|nzte-report</v>
+        <v>cancer|oncology|waiting-time|nzte-report</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>1225</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>19</v>
@@ -11697,13 +12257,25 @@
         <v>634</v>
       </c>
     </row>
-    <row r="131" spans="1:23" ht="409" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:23" ht="409" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>635</v>
       </c>
+      <c r="B131" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>1175</v>
+      </c>
       <c r="E131" s="1" t="str">
         <f t="shared" ref="E131:E194" si="2">CONCATENATE(F131, "|", "nzte-report")</f>
-        <v>|nzte-report</v>
+        <v>cancer|oncology|pulmonology|nzte-report</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>1331</v>
       </c>
       <c r="G131" s="1" t="s">
         <v>19</v>
@@ -11742,13 +12314,25 @@
         <v>643</v>
       </c>
     </row>
-    <row r="132" spans="1:23" ht="120" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:23" ht="120" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>644</v>
       </c>
+      <c r="B132" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>1175</v>
+      </c>
       <c r="E132" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>cancer|oncology|gastroenterology|nzte-report</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>1332</v>
       </c>
       <c r="G132" s="1" t="s">
         <v>19</v>
@@ -11784,13 +12368,25 @@
         <v>649</v>
       </c>
     </row>
-    <row r="133" spans="1:23" ht="180" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:23" ht="180" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>650</v>
       </c>
+      <c r="B133" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>1175</v>
+      </c>
       <c r="E133" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>cancer|oncology|gastroenterology|nzte-report</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>1332</v>
       </c>
       <c r="G133" s="1" t="s">
         <v>19</v>
@@ -11826,13 +12422,25 @@
         <v>655</v>
       </c>
     </row>
-    <row r="134" spans="1:23" ht="330" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:23" ht="330" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>656</v>
       </c>
+      <c r="B134" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>1175</v>
+      </c>
       <c r="E134" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>cancer|oncology|waiting-time|nzte-report</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>1225</v>
       </c>
       <c r="G134" s="1" t="s">
         <v>19</v>
@@ -11862,13 +12470,25 @@
         <v>661</v>
       </c>
     </row>
-    <row r="135" spans="1:23" ht="255" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:23" ht="255" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>662</v>
       </c>
+      <c r="B135" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>1175</v>
+      </c>
       <c r="E135" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>cancer|oncology|nzte-report</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>1217</v>
       </c>
       <c r="G135" s="1" t="s">
         <v>19</v>
@@ -11892,13 +12512,25 @@
         <v>665</v>
       </c>
     </row>
-    <row r="136" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>666</v>
       </c>
+      <c r="B136" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>1175</v>
+      </c>
       <c r="E136" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>cancer|oncology|nzte-report</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>1217</v>
       </c>
       <c r="G136" s="1" t="s">
         <v>19</v>
@@ -11916,13 +12548,25 @@
         <v>668</v>
       </c>
     </row>
-    <row r="137" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:23" ht="45" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>669</v>
       </c>
+      <c r="B137" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>1175</v>
+      </c>
       <c r="E137" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>cancer|oncology|nzte-report</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>1217</v>
       </c>
       <c r="G137" s="1" t="s">
         <v>19</v>
@@ -11937,13 +12581,25 @@
         <v>670</v>
       </c>
     </row>
-    <row r="138" spans="1:23" ht="90" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:23" ht="90" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>671</v>
       </c>
+      <c r="B138" s="1" t="s">
+        <v>1382</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>1381</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>1175</v>
+      </c>
       <c r="E138" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>cancer|oncology|gastroenterology|nzte-report</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>1332</v>
       </c>
       <c r="G138" s="1" t="s">
         <v>19</v>
@@ -11958,13 +12614,25 @@
         <v>673</v>
       </c>
     </row>
-    <row r="139" spans="1:23" ht="165" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:23" ht="165" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>674</v>
       </c>
+      <c r="B139" s="1" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>1383</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>1230</v>
+      </c>
       <c r="E139" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>global-health|nzte-report</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>1183</v>
       </c>
       <c r="G139" s="1" t="s">
         <v>258</v>
@@ -12018,13 +12686,25 @@
         <v>688</v>
       </c>
     </row>
-    <row r="140" spans="1:23" ht="90" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:23" ht="90" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>689</v>
       </c>
+      <c r="B140" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>1351</v>
+      </c>
       <c r="E140" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>laboratory|radiology|pharmacy|nzte-report</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>1386</v>
       </c>
       <c r="G140" s="1" t="s">
         <v>690</v>
@@ -12078,13 +12758,25 @@
         <v>701</v>
       </c>
     </row>
-    <row r="141" spans="1:23" ht="195" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:23" ht="195" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>702</v>
       </c>
+      <c r="B141" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>1175</v>
+      </c>
       <c r="E141" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>cancer|oncology|nzte-report</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>1217</v>
       </c>
       <c r="G141" s="1" t="s">
         <v>444</v>
@@ -12186,13 +12878,25 @@
         <v>721</v>
       </c>
     </row>
-    <row r="143" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>722</v>
       </c>
+      <c r="B143" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>1388</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>1256</v>
+      </c>
       <c r="E143" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>rheumatology|nzte-report</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>1387</v>
       </c>
       <c r="G143" s="1" t="s">
         <v>444</v>
@@ -12207,13 +12911,25 @@
         <v>722</v>
       </c>
     </row>
-    <row r="144" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>723</v>
       </c>
+      <c r="B144" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>1175</v>
+      </c>
       <c r="E144" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>gp|primary-care|nzte-report</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>1288</v>
       </c>
       <c r="G144" s="1" t="s">
         <v>19</v>
@@ -12264,16 +12980,25 @@
         <v>736</v>
       </c>
     </row>
-    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>737</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>1302</v>
       </c>
+      <c r="C145" s="1" t="s">
+        <v>1304</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>1175</v>
+      </c>
       <c r="E145" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>primary-care|nzte-report</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>1214</v>
       </c>
       <c r="G145" s="1" t="s">
         <v>19</v>
@@ -13116,7 +13841,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="169" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>765</v>
       </c>
@@ -13131,7 +13856,10 @@
       </c>
       <c r="E169" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>hospital|nzte-report</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>1299</v>
       </c>
       <c r="G169" s="1" t="s">
         <v>254</v>
@@ -13185,7 +13913,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="171" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>767</v>
       </c>
@@ -13200,7 +13928,10 @@
       </c>
       <c r="E171" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>hospital|nzte-report</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>1299</v>
       </c>
       <c r="G171" s="1" t="s">
         <v>254</v>
@@ -13326,13 +14057,25 @@
         <v>770</v>
       </c>
     </row>
-    <row r="175" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>771</v>
       </c>
+      <c r="B175" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E175" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>emergency|hospital|nzte-report</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>1335</v>
       </c>
       <c r="G175" s="1" t="s">
         <v>254</v>
@@ -13362,13 +14105,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="176" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>776</v>
       </c>
+      <c r="B176" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E176" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>inpatient|hospital|nzte-report</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>1336</v>
       </c>
       <c r="G176" s="1" t="s">
         <v>254</v>
@@ -13395,13 +14150,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="177" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>778</v>
       </c>
+      <c r="B177" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E177" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>outpatient|hospital|nzte-report</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>1337</v>
       </c>
       <c r="G177" s="1" t="s">
         <v>254</v>
@@ -13428,13 +14195,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="178" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>780</v>
       </c>
+      <c r="B178" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E178" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>theatre|hospital|nzte-report</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>1301</v>
       </c>
       <c r="G178" s="1" t="s">
         <v>254</v>
@@ -13461,13 +14240,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="179" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>782</v>
       </c>
+      <c r="B179" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E179" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>waiting-time|hospital|nzte-report</v>
+      </c>
+      <c r="F179" s="1" t="s">
+        <v>1338</v>
       </c>
       <c r="G179" s="1" t="s">
         <v>254</v>
@@ -13494,13 +14285,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="180" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>783</v>
       </c>
+      <c r="B180" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E180" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>hospital|nzte-report</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>1299</v>
       </c>
       <c r="G180" s="1" t="s">
         <v>254</v>
@@ -13527,13 +14330,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="181" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>784</v>
       </c>
+      <c r="B181" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E181" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>hospital|nzte-report</v>
+      </c>
+      <c r="F181" s="1" t="s">
+        <v>1299</v>
       </c>
       <c r="G181" s="1" t="s">
         <v>254</v>
@@ -13560,13 +14375,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="182" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>785</v>
       </c>
+      <c r="B182" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E182" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>hospital|nzte-report</v>
+      </c>
+      <c r="F182" s="1" t="s">
+        <v>1299</v>
       </c>
       <c r="G182" s="1" t="s">
         <v>254</v>
@@ -13593,13 +14420,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="183" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>786</v>
       </c>
+      <c r="B183" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E183" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>hospital|nzte-report</v>
+      </c>
+      <c r="F183" s="1" t="s">
+        <v>1299</v>
       </c>
       <c r="G183" s="1" t="s">
         <v>254</v>
@@ -13626,13 +14465,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="184" spans="1:22" ht="75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:22" ht="75" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>787</v>
       </c>
+      <c r="B184" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E184" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>rehabilitation|hospital|nzte-report</v>
+      </c>
+      <c r="F184" s="1" t="s">
+        <v>1339</v>
       </c>
       <c r="G184" s="1" t="s">
         <v>254</v>
@@ -13659,13 +14510,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="185" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>789</v>
       </c>
+      <c r="B185" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E185" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>mental-health|hospital|nzte-report</v>
+      </c>
+      <c r="F185" s="1" t="s">
+        <v>1340</v>
       </c>
       <c r="G185" s="1" t="s">
         <v>254</v>
@@ -13692,13 +14555,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="186" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>791</v>
       </c>
+      <c r="B186" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E186" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>image|hospital|nzte-report</v>
+      </c>
+      <c r="F186" s="1" t="s">
+        <v>1347</v>
       </c>
       <c r="G186" s="1" t="s">
         <v>254</v>
@@ -13725,13 +14600,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="187" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>792</v>
       </c>
+      <c r="B187" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E187" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>hospital|nzte-report</v>
+      </c>
+      <c r="F187" s="1" t="s">
+        <v>1299</v>
       </c>
       <c r="G187" s="1" t="s">
         <v>254</v>
@@ -13758,13 +14645,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="188" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>794</v>
       </c>
+      <c r="B188" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E188" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>pediatrics|hospital|nzte-report</v>
+      </c>
+      <c r="F188" s="1" t="s">
+        <v>1346</v>
       </c>
       <c r="G188" s="1" t="s">
         <v>254</v>
@@ -13791,13 +14690,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="189" spans="1:22" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:22" ht="60" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>796</v>
       </c>
+      <c r="B189" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E189" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>hospital|nzte-report</v>
+      </c>
+      <c r="F189" s="1" t="s">
+        <v>1299</v>
       </c>
       <c r="G189" s="1" t="s">
         <v>254</v>
@@ -13824,13 +14735,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="190" spans="1:22" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:22" ht="45" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>797</v>
       </c>
+      <c r="B190" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E190" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>elderly|hospital|nzte-report</v>
+      </c>
+      <c r="F190" s="1" t="s">
+        <v>1345</v>
       </c>
       <c r="G190" s="1" t="s">
         <v>254</v>
@@ -13857,13 +14780,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="191" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>799</v>
       </c>
+      <c r="B191" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E191" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>mental-health|hospital|nzte-report</v>
+      </c>
+      <c r="F191" s="1" t="s">
+        <v>1340</v>
       </c>
       <c r="G191" s="1" t="s">
         <v>254</v>
@@ -13890,13 +14825,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="192" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>800</v>
       </c>
+      <c r="B192" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E192" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>hospital|nzte-report</v>
+      </c>
+      <c r="F192" s="1" t="s">
+        <v>1299</v>
       </c>
       <c r="G192" s="1" t="s">
         <v>254</v>
@@ -13923,13 +14870,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="193" spans="1:23" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:23" ht="60" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>801</v>
       </c>
+      <c r="B193" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E193" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>mental-health|hospital|nzte-report</v>
+      </c>
+      <c r="F193" s="1" t="s">
+        <v>1340</v>
       </c>
       <c r="G193" s="1" t="s">
         <v>254</v>
@@ -13956,13 +14915,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="194" spans="1:23" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:23" ht="60" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>802</v>
       </c>
+      <c r="B194" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E194" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|nzte-report</v>
+        <v>hospital|referral|nzte-report</v>
+      </c>
+      <c r="F194" s="1" t="s">
+        <v>1341</v>
       </c>
       <c r="G194" s="1" t="s">
         <v>254</v>
@@ -13989,13 +14960,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="195" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:23" ht="45" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>804</v>
       </c>
+      <c r="B195" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E195" s="1" t="str">
         <f t="shared" ref="E195:E258" si="3">CONCATENATE(F195, "|", "nzte-report")</f>
-        <v>|nzte-report</v>
+        <v>hospital|nzte-report</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>1299</v>
       </c>
       <c r="G195" s="1" t="s">
         <v>254</v>
@@ -14022,13 +15005,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="196" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>805</v>
       </c>
+      <c r="B196" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E196" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>hospital|nzte-report</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>1299</v>
       </c>
       <c r="G196" s="1" t="s">
         <v>254</v>
@@ -14055,13 +15050,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="197" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>806</v>
       </c>
+      <c r="B197" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E197" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>medication|hospital|nzte-report</v>
+      </c>
+      <c r="F197" s="1" t="s">
+        <v>1343</v>
       </c>
       <c r="G197" s="1" t="s">
         <v>254</v>
@@ -14088,13 +15095,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="198" spans="1:23" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:23" ht="60" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>807</v>
       </c>
+      <c r="B198" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E198" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>hospital|nzte-report</v>
+      </c>
+      <c r="F198" s="1" t="s">
+        <v>1299</v>
       </c>
       <c r="G198" s="1" t="s">
         <v>254</v>
@@ -14121,13 +15140,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="199" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>809</v>
       </c>
+      <c r="B199" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E199" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>ambulance|hospital|nzte-report</v>
+      </c>
+      <c r="F199" s="1" t="s">
+        <v>1344</v>
       </c>
       <c r="G199" s="1" t="s">
         <v>254</v>
@@ -14154,13 +15185,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="200" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:23" ht="45" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>812</v>
       </c>
+      <c r="B200" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>1228</v>
+      </c>
       <c r="E200" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>hospital|nzte-report</v>
+      </c>
+      <c r="F200" s="1" t="s">
+        <v>1299</v>
       </c>
       <c r="G200" s="1" t="s">
         <v>254</v>
@@ -15375,13 +16418,25 @@
         <v>825</v>
       </c>
     </row>
-    <row r="221" spans="1:23" ht="120" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:23" ht="120" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>872</v>
       </c>
+      <c r="B221" s="1" t="s">
+        <v>1353</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>1352</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>1351</v>
+      </c>
       <c r="E221" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>laboratory|nzte-report</v>
+      </c>
+      <c r="F221" s="1" t="s">
+        <v>1237</v>
       </c>
       <c r="G221" s="1" t="s">
         <v>690</v>
@@ -15432,13 +16487,25 @@
         <v>885</v>
       </c>
     </row>
-    <row r="222" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>886</v>
       </c>
+      <c r="B222" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>1389</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>1351</v>
+      </c>
       <c r="E222" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>laboratory|image|nzte-report</v>
+      </c>
+      <c r="F222" s="1" t="s">
+        <v>1390</v>
       </c>
       <c r="G222" s="1" t="s">
         <v>690</v>
@@ -15453,13 +16520,25 @@
         <v>725</v>
       </c>
     </row>
-    <row r="223" spans="1:23" ht="165" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:23" ht="165" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>887</v>
       </c>
+      <c r="B223" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>1375</v>
+      </c>
       <c r="E223" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>primary-care|gp|nzte-report</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>1235</v>
       </c>
       <c r="G223" s="1" t="s">
         <v>380</v>
@@ -15510,13 +16589,25 @@
         <v>898</v>
       </c>
     </row>
-    <row r="224" spans="1:23" ht="75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:23" ht="75" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>899</v>
       </c>
+      <c r="B224" s="1" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>1375</v>
+      </c>
       <c r="E224" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>primary-care|claim|nzte-report</v>
+      </c>
+      <c r="F224" s="1" t="s">
+        <v>1392</v>
       </c>
       <c r="G224" s="1" t="s">
         <v>380</v>
@@ -15549,13 +16640,25 @@
         <v>905</v>
       </c>
     </row>
-    <row r="225" spans="1:23" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:23" ht="60" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>906</v>
       </c>
+      <c r="B225" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>1393</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>1375</v>
+      </c>
       <c r="E225" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>nurse|home-care|nzte-report</v>
+      </c>
+      <c r="F225" s="1" t="s">
+        <v>1394</v>
       </c>
       <c r="G225" s="1" t="s">
         <v>380</v>
@@ -15582,13 +16685,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="226" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:23" ht="45" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>909</v>
       </c>
+      <c r="B226" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>1393</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>1375</v>
+      </c>
       <c r="E226" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>nurse|home-care|nzte-report</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>1394</v>
       </c>
       <c r="G226" s="1" t="s">
         <v>380</v>
@@ -15615,13 +16730,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="227" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:23" ht="45" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>910</v>
       </c>
+      <c r="B227" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>1393</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>1375</v>
+      </c>
       <c r="E227" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>nurse|home-care|nzte-report</v>
+      </c>
+      <c r="F227" s="1" t="s">
+        <v>1394</v>
       </c>
       <c r="G227" s="1" t="s">
         <v>380</v>
@@ -15648,13 +16775,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="228" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:23" ht="45" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>911</v>
       </c>
+      <c r="B228" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>1393</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>1375</v>
+      </c>
       <c r="E228" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>nurse|home-care|nzte-report</v>
+      </c>
+      <c r="F228" s="1" t="s">
+        <v>1394</v>
       </c>
       <c r="G228" s="1" t="s">
         <v>380</v>
@@ -15681,13 +16820,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="229" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>912</v>
       </c>
+      <c r="B229" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>1393</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>1375</v>
+      </c>
       <c r="E229" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>nurse|home-care|nzte-report</v>
+      </c>
+      <c r="F229" s="1" t="s">
+        <v>1394</v>
       </c>
       <c r="G229" s="1" t="s">
         <v>380</v>
@@ -15714,13 +16865,25 @@
         <v>775</v>
       </c>
     </row>
-    <row r="230" spans="1:23" ht="120" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:23" ht="120" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>914</v>
       </c>
+      <c r="B230" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>1350</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E230" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>diabetes|nzte-report</v>
+      </c>
+      <c r="F230" s="1" t="s">
+        <v>1189</v>
       </c>
       <c r="G230" s="1" t="s">
         <v>394</v>
@@ -15840,13 +17003,25 @@
         <v>939</v>
       </c>
     </row>
-    <row r="232" spans="1:23" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:23" ht="60" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>940</v>
       </c>
+      <c r="B232" s="1" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>1395</v>
+      </c>
+      <c r="D232" s="1" t="s">
+        <v>1256</v>
+      </c>
       <c r="E232" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>global-health|nzte-report</v>
+      </c>
+      <c r="F232" s="1" t="s">
+        <v>1183</v>
       </c>
       <c r="G232" s="1" t="s">
         <v>444</v>
@@ -15885,13 +17060,25 @@
         <v>65</v>
       </c>
     </row>
-    <row r="233" spans="1:23" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:23" ht="60" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>944</v>
       </c>
+      <c r="B233" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D233" s="1" t="s">
+        <v>1256</v>
+      </c>
       <c r="E233" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>pediatrics|nzte-report</v>
+      </c>
+      <c r="F233" s="1" t="s">
+        <v>1184</v>
       </c>
       <c r="G233" s="1" t="s">
         <v>444</v>
@@ -15963,13 +17150,25 @@
         <v>947</v>
       </c>
     </row>
-    <row r="235" spans="1:23" ht="150" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:23" ht="150" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>948</v>
       </c>
+      <c r="B235" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>1350</v>
+      </c>
+      <c r="D235" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E235" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>diabetes|nzte-report</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>1189</v>
       </c>
       <c r="G235" s="1" t="s">
         <v>394</v>
@@ -16020,13 +17219,25 @@
         <v>960</v>
       </c>
     </row>
-    <row r="236" spans="1:23" ht="120" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:23" ht="120" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>961</v>
       </c>
+      <c r="B236" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>1350</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E236" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>diabetes|nzte-report</v>
+      </c>
+      <c r="F236" s="1" t="s">
+        <v>1189</v>
       </c>
       <c r="G236" s="1" t="s">
         <v>394</v>
@@ -16074,13 +17285,25 @@
         <v>968</v>
       </c>
     </row>
-    <row r="237" spans="1:23" ht="255" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:23" ht="255" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>969</v>
       </c>
+      <c r="B237" s="1" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>1356</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E237" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>cardiology|nzte-report</v>
+      </c>
+      <c r="F237" s="1" t="s">
+        <v>1205</v>
       </c>
       <c r="G237" s="1" t="s">
         <v>394</v>
@@ -16131,13 +17354,25 @@
         <v>980</v>
       </c>
     </row>
-    <row r="238" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>981</v>
       </c>
+      <c r="B238" s="1" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>1364</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E238" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>pediatrics|nzte-report</v>
+      </c>
+      <c r="F238" s="1" t="s">
+        <v>1184</v>
       </c>
       <c r="G238" s="1" t="s">
         <v>394</v>
@@ -16191,13 +17426,25 @@
         <v>995</v>
       </c>
     </row>
-    <row r="239" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>996</v>
       </c>
+      <c r="B239" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E239" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>cardiology|nzte-report</v>
+      </c>
+      <c r="F239" s="1" t="s">
+        <v>1205</v>
       </c>
       <c r="G239" s="1" t="s">
         <v>394</v>
@@ -16224,13 +17471,25 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="240" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:23" ht="45" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>1001</v>
       </c>
+      <c r="B240" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E240" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>cardiology|nzte-report</v>
+      </c>
+      <c r="F240" s="1" t="s">
+        <v>1205</v>
       </c>
       <c r="G240" s="1" t="s">
         <v>394</v>
@@ -16257,13 +17516,25 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="241" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>1006</v>
       </c>
+      <c r="B241" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D241" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E241" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>blood-donation|nzte-report</v>
+      </c>
+      <c r="F241" s="1" t="s">
+        <v>1398</v>
       </c>
       <c r="G241" s="1" t="s">
         <v>394</v>
@@ -16287,13 +17558,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="242" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>1009</v>
       </c>
+      <c r="B242" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E242" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>radiology|nzte-report</v>
+      </c>
+      <c r="F242" s="1" t="s">
+        <v>1201</v>
       </c>
       <c r="G242" s="1" t="s">
         <v>394</v>
@@ -16317,13 +17600,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="243" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>1013</v>
       </c>
+      <c r="B243" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E243" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>cardiology|nzte-report</v>
+      </c>
+      <c r="F243" s="1" t="s">
+        <v>1205</v>
       </c>
       <c r="G243" s="1" t="s">
         <v>394</v>
@@ -16347,13 +17642,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="244" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>1017</v>
       </c>
+      <c r="B244" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E244" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>tobacco|smoking|addiction|nzte-report</v>
+      </c>
+      <c r="F244" s="1" t="s">
+        <v>1399</v>
       </c>
       <c r="G244" s="1" t="s">
         <v>394</v>
@@ -16377,13 +17684,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="245" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>1021</v>
       </c>
+      <c r="B245" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E245" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>cholesterol|nzte-report</v>
+      </c>
+      <c r="F245" s="1" t="s">
+        <v>1400</v>
       </c>
       <c r="G245" s="1" t="s">
         <v>394</v>
@@ -16407,13 +17726,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="246" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>1021</v>
       </c>
+      <c r="B246" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E246" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>research|nzte-report</v>
+      </c>
+      <c r="F246" s="1" t="s">
+        <v>1409</v>
       </c>
       <c r="G246" s="1" t="s">
         <v>394</v>
@@ -16437,13 +17768,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="247" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
         <v>1025</v>
       </c>
+      <c r="B247" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E247" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>tobacco|smoking|addiction|nzte-report</v>
+      </c>
+      <c r="F247" s="1" t="s">
+        <v>1399</v>
       </c>
       <c r="G247" s="1" t="s">
         <v>394</v>
@@ -16467,13 +17810,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="248" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>1028</v>
       </c>
+      <c r="B248" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E248" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>tobacco|smoking|addiction|nzte-report</v>
+      </c>
+      <c r="F248" s="1" t="s">
+        <v>1399</v>
       </c>
       <c r="G248" s="1" t="s">
         <v>394</v>
@@ -16497,13 +17852,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="249" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
         <v>1032</v>
       </c>
+      <c r="B249" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E249" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>nutrition|nzte-report</v>
+      </c>
+      <c r="F249" s="1" t="s">
+        <v>1267</v>
       </c>
       <c r="G249" s="1" t="s">
         <v>394</v>
@@ -16527,13 +17894,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="250" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
         <v>1036</v>
       </c>
+      <c r="B250" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E250" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>stroke|nzte-report</v>
+      </c>
+      <c r="F250" s="1" t="s">
+        <v>1401</v>
       </c>
       <c r="G250" s="1" t="s">
         <v>394</v>
@@ -16557,13 +17936,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="251" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
         <v>1040</v>
       </c>
+      <c r="B251" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E251" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>tobacco|smoking|addiction|nzte-report</v>
+      </c>
+      <c r="F251" s="1" t="s">
+        <v>1399</v>
       </c>
       <c r="G251" s="1" t="s">
         <v>394</v>
@@ -16587,13 +17978,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="252" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
         <v>1044</v>
       </c>
+      <c r="B252" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E252" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>social|research|qol|lifstyle|nzte-report</v>
+      </c>
+      <c r="F252" s="1" t="s">
+        <v>1411</v>
       </c>
       <c r="G252" s="1" t="s">
         <v>394</v>
@@ -16617,13 +18020,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="253" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
         <v>1048</v>
       </c>
+      <c r="B253" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E253" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>tobacco|smoking|cardiology|nzte-report</v>
+      </c>
+      <c r="F253" s="1" t="s">
+        <v>1402</v>
       </c>
       <c r="G253" s="1" t="s">
         <v>394</v>
@@ -16647,13 +18062,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="254" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
         <v>1052</v>
       </c>
+      <c r="B254" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E254" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>research|nzte-report</v>
+      </c>
+      <c r="F254" s="1" t="s">
+        <v>1409</v>
       </c>
       <c r="G254" s="1" t="s">
         <v>394</v>
@@ -16677,13 +18104,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="255" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
         <v>1054</v>
       </c>
+      <c r="B255" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E255" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>mental-health|hospital|nzte-report</v>
+      </c>
+      <c r="F255" s="1" t="s">
+        <v>1340</v>
       </c>
       <c r="G255" s="1" t="s">
         <v>394</v>
@@ -16707,13 +18146,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="256" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
         <v>1058</v>
       </c>
+      <c r="B256" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D256" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E256" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>nutrition|nzte-report</v>
+      </c>
+      <c r="F256" s="1" t="s">
+        <v>1267</v>
       </c>
       <c r="G256" s="1" t="s">
         <v>394</v>
@@ -16737,13 +18188,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="257" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
         <v>1062</v>
       </c>
+      <c r="B257" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E257" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>tobacco|smoking|addiction|alcohol|nzte-report</v>
+      </c>
+      <c r="F257" s="1" t="s">
+        <v>1403</v>
       </c>
       <c r="G257" s="1" t="s">
         <v>394</v>
@@ -16767,13 +18230,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="258" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
         <v>1066</v>
       </c>
+      <c r="B258" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E258" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>|nzte-report</v>
+        <v>barthel-index|research|adl|nzte-report</v>
+      </c>
+      <c r="F258" s="1" t="s">
+        <v>1412</v>
       </c>
       <c r="G258" s="1" t="s">
         <v>394</v>
@@ -16797,13 +18272,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="259" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
         <v>1070</v>
       </c>
+      <c r="B259" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D259" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E259" s="1" t="str">
         <f t="shared" ref="E259:E287" si="4">CONCATENATE(F259, "|", "nzte-report")</f>
-        <v>|nzte-report</v>
+        <v>qol|research|cardiology|nzte-report</v>
+      </c>
+      <c r="F259" s="1" t="s">
+        <v>1413</v>
       </c>
       <c r="G259" s="1" t="s">
         <v>394</v>
@@ -16827,13 +18314,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="260" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
         <v>1074</v>
       </c>
+      <c r="B260" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E260" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>tobacco|smoking|addiction|nzte-report</v>
+      </c>
+      <c r="F260" s="1" t="s">
+        <v>1399</v>
       </c>
       <c r="G260" s="1" t="s">
         <v>394</v>
@@ -16857,13 +18356,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="261" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
         <v>1078</v>
       </c>
+      <c r="B261" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D261" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E261" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>freemasons|research|nzte-report</v>
+      </c>
+      <c r="F261" s="1" t="s">
+        <v>1414</v>
       </c>
       <c r="G261" s="1" t="s">
         <v>394</v>
@@ -16887,13 +18398,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="262" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="s">
         <v>1080</v>
       </c>
+      <c r="B262" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E262" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>car-crash|nzte-report</v>
+      </c>
+      <c r="F262" s="1" t="s">
+        <v>1404</v>
       </c>
       <c r="G262" s="1" t="s">
         <v>394</v>
@@ -16917,13 +18440,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="263" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
         <v>1082</v>
       </c>
+      <c r="B263" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D263" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E263" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>stroke|nzte-report</v>
+      </c>
+      <c r="F263" s="1" t="s">
+        <v>1401</v>
       </c>
       <c r="G263" s="1" t="s">
         <v>394</v>
@@ -16947,13 +18482,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="264" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
         <v>1085</v>
       </c>
+      <c r="B264" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D264" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E264" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>sleep|nzte-report</v>
+      </c>
+      <c r="F264" s="1" t="s">
+        <v>1405</v>
       </c>
       <c r="G264" s="1" t="s">
         <v>394</v>
@@ -16977,13 +18524,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="265" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
         <v>1089</v>
       </c>
+      <c r="B265" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D265" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E265" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>mental-health|nzte-report</v>
+      </c>
+      <c r="F265" s="1" t="s">
+        <v>1204</v>
       </c>
       <c r="G265" s="1" t="s">
         <v>394</v>
@@ -17007,13 +18566,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="266" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
         <v>1093</v>
       </c>
+      <c r="B266" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D266" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E266" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>nutrition|nzte-report</v>
+      </c>
+      <c r="F266" s="1" t="s">
+        <v>1267</v>
       </c>
       <c r="G266" s="1" t="s">
         <v>394</v>
@@ -17037,13 +18608,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="267" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="s">
         <v>1097</v>
       </c>
+      <c r="B267" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D267" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E267" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>steroid|research|nzte-report</v>
+      </c>
+      <c r="F267" s="1" t="s">
+        <v>1415</v>
       </c>
       <c r="G267" s="1" t="s">
         <v>394</v>
@@ -17067,13 +18650,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="268" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
         <v>1099</v>
       </c>
+      <c r="B268" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D268" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E268" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>qol|research|nzte-report</v>
+      </c>
+      <c r="F268" s="1" t="s">
+        <v>1416</v>
       </c>
       <c r="G268" s="1" t="s">
         <v>394</v>
@@ -17097,13 +18692,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="269" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
         <v>1103</v>
       </c>
+      <c r="B269" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D269" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E269" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>radiology|research|nzte-report</v>
+      </c>
+      <c r="F269" s="1" t="s">
+        <v>1417</v>
       </c>
       <c r="G269" s="1" t="s">
         <v>394</v>
@@ -17127,13 +18734,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="270" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A270" s="1" t="s">
         <v>1105</v>
       </c>
+      <c r="B270" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D270" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E270" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>blood-donation|nzte-report</v>
+      </c>
+      <c r="F270" s="1" t="s">
+        <v>1398</v>
       </c>
       <c r="G270" s="1" t="s">
         <v>394</v>
@@ -17157,13 +18776,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="271" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A271" s="1" t="s">
         <v>1107</v>
       </c>
+      <c r="B271" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D271" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E271" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>ulcer|medication|nzte-report</v>
+      </c>
+      <c r="F271" s="1" t="s">
+        <v>1406</v>
       </c>
       <c r="G271" s="1" t="s">
         <v>394</v>
@@ -17187,13 +18818,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="272" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A272" s="1" t="s">
         <v>1111</v>
       </c>
+      <c r="B272" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D272" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E272" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>nephrology|nzte-report</v>
+      </c>
+      <c r="F272" s="1" t="s">
+        <v>1315</v>
       </c>
       <c r="G272" s="1" t="s">
         <v>394</v>
@@ -17217,13 +18860,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="273" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A273" s="1" t="s">
         <v>1115</v>
       </c>
+      <c r="B273" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D273" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E273" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>sport|global-health|nzte-report</v>
+      </c>
+      <c r="F273" s="1" t="s">
+        <v>1407</v>
       </c>
       <c r="G273" s="1" t="s">
         <v>394</v>
@@ -17247,13 +18902,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="274" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
         <v>1119</v>
       </c>
+      <c r="B274" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D274" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E274" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>nutrition|nzte-report</v>
+      </c>
+      <c r="F274" s="1" t="s">
+        <v>1267</v>
       </c>
       <c r="G274" s="1" t="s">
         <v>394</v>
@@ -17277,13 +18944,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="275" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A275" s="1" t="s">
         <v>1122</v>
       </c>
+      <c r="B275" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D275" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E275" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>adherence|research|nzte-report</v>
+      </c>
+      <c r="F275" s="1" t="s">
+        <v>1418</v>
       </c>
       <c r="G275" s="1" t="s">
         <v>394</v>
@@ -17307,13 +18986,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="276" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
         <v>1126</v>
       </c>
+      <c r="B276" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D276" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E276" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>medication|nzte-report</v>
+      </c>
+      <c r="F276" s="1" t="s">
+        <v>1342</v>
       </c>
       <c r="G276" s="1" t="s">
         <v>394</v>
@@ -17337,13 +19028,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="277" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A277" s="1" t="s">
         <v>1130</v>
       </c>
+      <c r="B277" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E277" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>social|research|nzte-report</v>
+      </c>
+      <c r="F277" s="1" t="s">
+        <v>1410</v>
       </c>
       <c r="G277" s="1" t="s">
         <v>394</v>
@@ -17367,13 +19070,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="278" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
         <v>1134</v>
       </c>
+      <c r="B278" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D278" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E278" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>asthma|nzte-report</v>
+      </c>
+      <c r="F278" s="1" t="s">
+        <v>1408</v>
       </c>
       <c r="G278" s="1" t="s">
         <v>394</v>
@@ -17397,13 +19112,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="279" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A279" s="1" t="s">
         <v>1138</v>
       </c>
+      <c r="B279" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D279" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E279" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>nutrition|research|nzte-report</v>
+      </c>
+      <c r="F279" s="1" t="s">
+        <v>1419</v>
       </c>
       <c r="G279" s="1" t="s">
         <v>394</v>
@@ -17427,13 +19154,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="280" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
         <v>1142</v>
       </c>
+      <c r="B280" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E280" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>stroke|nzte-report</v>
+      </c>
+      <c r="F280" s="1" t="s">
+        <v>1401</v>
       </c>
       <c r="G280" s="1" t="s">
         <v>394</v>
@@ -17457,13 +19196,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="281" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A281" s="1" t="s">
         <v>1146</v>
       </c>
+      <c r="B281" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D281" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E281" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>research|nzte-report</v>
+      </c>
+      <c r="F281" s="1" t="s">
+        <v>1409</v>
       </c>
       <c r="G281" s="1" t="s">
         <v>394</v>
@@ -17487,13 +19238,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="282" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A282" s="1" t="s">
         <v>1148</v>
       </c>
+      <c r="B282" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D282" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E282" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>addiction|research|nzte-report</v>
+      </c>
+      <c r="F282" s="1" t="s">
+        <v>1420</v>
       </c>
       <c r="G282" s="1" t="s">
         <v>394</v>
@@ -17517,13 +19280,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="283" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A283" s="1" t="s">
         <v>1152</v>
       </c>
+      <c r="B283" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E283" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>stroke|nzte-report</v>
+      </c>
+      <c r="F283" s="1" t="s">
+        <v>1401</v>
       </c>
       <c r="G283" s="1" t="s">
         <v>394</v>
@@ -17547,13 +19322,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="284" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A284" s="1" t="s">
         <v>1154</v>
       </c>
+      <c r="B284" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D284" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E284" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>adherence|research|nzte-report</v>
+      </c>
+      <c r="F284" s="1" t="s">
+        <v>1418</v>
       </c>
       <c r="G284" s="1" t="s">
         <v>394</v>
@@ -17577,13 +19364,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="285" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A285" s="1" t="s">
         <v>1158</v>
       </c>
+      <c r="B285" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D285" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E285" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>sport|lifestyle|research|nzte-report</v>
+      </c>
+      <c r="F285" s="1" t="s">
+        <v>1421</v>
       </c>
       <c r="G285" s="1" t="s">
         <v>394</v>
@@ -17607,13 +19406,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="286" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A286" s="1" t="s">
         <v>1162</v>
       </c>
+      <c r="B286" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D286" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E286" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>qol|research|nzte-report</v>
+      </c>
+      <c r="F286" s="1" t="s">
+        <v>1416</v>
       </c>
       <c r="G286" s="1" t="s">
         <v>394</v>
@@ -17637,13 +19448,25 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="287" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:23" ht="105" x14ac:dyDescent="0.2">
       <c r="A287" s="1" t="s">
         <v>1166</v>
       </c>
+      <c r="B287" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D287" s="1" t="s">
+        <v>1303</v>
+      </c>
       <c r="E287" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>|nzte-report</v>
+        <v>nutrition|nzte-report</v>
+      </c>
+      <c r="F287" s="1" t="s">
+        <v>1267</v>
       </c>
       <c r="G287" s="1" t="s">
         <v>394</v>
@@ -17665,93 +19488,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W287">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="acc|nzte-report"/>
-        <filter val="addiction|gambling|nzte-report"/>
-        <filter val="alcohol|addiction|drug-use|nzte-report"/>
-        <filter val="assistance|nzte-report"/>
-        <filter val="awareness|nzte-report"/>
-        <filter val="cancer|nzte-report"/>
-        <filter val="cancer|oncology|nzte-report"/>
-        <filter val="cancer|oncology|waiting-time|nzte-report"/>
-        <filter val="cardiology|nzte-report"/>
-        <filter val="claims|mental-health|addiction|nzte-report"/>
-        <filter val="compliance|nzte-report"/>
-        <filter val="costing|nzte-report"/>
-        <filter val="dhb|nzte-report"/>
-        <filter val="diabetes|cardiology|nzte-report"/>
-        <filter val="diabetes|nzte-report"/>
-        <filter val="diet|nzte-report"/>
-        <filter val="discharge|nzte-report"/>
-        <filter val="drugs|awareness|nzte-report"/>
-        <filter val="drugs|nzte-report"/>
-        <filter val="elderly|nzte-report"/>
-        <filter val="elderly|residential-care|nzte-report"/>
-        <filter val="emergency|nzte-report"/>
-        <filter val="examination|nzte-report"/>
-        <filter val="gastroenterology|nzte-report"/>
-        <filter val="global-health|nzte-report"/>
-        <filter val="gp|primary-care|nzte-report"/>
-        <filter val="gynaecology|nzte-report"/>
-        <filter val="hiv|nzte-report"/>
-        <filter val="hospital|finance|nzte-report"/>
-        <filter val="hospital|nzte-report"/>
-        <filter val="hospital|theatre|nzte-report"/>
-        <filter val="hospital|trial|nzte-report"/>
-        <filter val="hospital|workforce|nzte-report"/>
-        <filter val="image|nzte-report"/>
-        <filter val="immunisation|nzte-report"/>
-        <filter val="instrument|nzte-report"/>
-        <filter val="laboratory|nzte-report"/>
-        <filter val="maori|nzte-report"/>
-        <filter val="maternity|nzte-report"/>
-        <filter val="mental-health|addiction|nzte-report"/>
-        <filter val="mental-health|nzte-report"/>
-        <filter val="mortality|nzte-report"/>
-        <filter val="nephrology|nzte-report"/>
-        <filter val="nurse|nzte-report"/>
-        <filter val="nutrition|nzte-report"/>
-        <filter val="oral|nzte-report"/>
-        <filter val="orthopaedics|nzte-report"/>
-        <filter val="outpatient|nzte-report"/>
-        <filter val="parenting|nurse|nzte-report"/>
-        <filter val="pediatrics|nutrition|nzte-report"/>
-        <filter val="pediatrics|nzte-report"/>
-        <filter val="pediatrics|school|nzte-report"/>
-        <filter val="pharmacy|nzte-report"/>
-        <filter val="primary-care|gp|nzte-report"/>
-        <filter val="primary-care|nzte-report"/>
-        <filter val="prisoners|nzte-report"/>
-        <filter val="radiology|nzte-report"/>
-        <filter val="radiology|waiting-time|nzte-report"/>
-        <filter val="school|nutrition|nzte-report"/>
-        <filter val="school|nzte-report"/>
-        <filter val="screening|nzte-report"/>
-        <filter val="secondary-care|nzte-report"/>
-        <filter val="smoking|primary-care|tobacco|nzte-report"/>
-        <filter val="smoking|tobacco|nzte-report"/>
-        <filter val="specialty|treatment|surgery|nzte-report"/>
-        <filter val="sport|nzte-report"/>
-        <filter val="surgery|nzte-report"/>
-        <filter val="theatre|hospital|nzte-report"/>
-        <filter val="tobacco|smoking|nzte-report"/>
-        <filter val="waiting-time|nzte-report"/>
-        <filter val="workforce|nzte-report"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="7">
-      <filters>
-        <filter val="ADHB"/>
-        <filter val="CMDHB"/>
-        <filter val="MoH"/>
-        <filter val="Southern DHB"/>
-        <filter val="Waikato DHB"/>
-        <filter val="WDHB"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>